<commit_message>
ADD purchase orders layer and modify providers
</commit_message>
<xml_diff>
--- a/worksheets/providers.xlsx
+++ b/worksheets/providers.xlsx
@@ -410,13 +410,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y3"/>
+  <dimension ref="A1:AMJ3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Z20" activeCellId="0" sqref="Z20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="20.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="21.17"/>
@@ -436,6 +436,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="18.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="13.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="21.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -514,6 +515,7 @@
       <c r="Y1" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -662,6 +664,7 @@
       <c r="Y3" s="5" t="s">
         <v>48</v>
       </c>
+      <c r="AMJ3" s="0"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>